<commit_message>
updated test case 2.1, 2.2
</commit_message>
<xml_diff>
--- a/guess_the_number_test_cases.xlsx
+++ b/guess_the_number_test_cases.xlsx
@@ -124,12 +124,6 @@
     <t>Print secret_num in new_game() to view answer. Input  following scenarios:</t>
   </si>
   <si>
-    <t>Incorrect guess: numeric. Guesses&gt;0</t>
-  </si>
-  <si>
-    <t>incorrect guess non-numeric (including blank)</t>
-  </si>
-  <si>
     <t>losing message is displayed</t>
   </si>
   <si>
@@ -140,6 +134,12 @@
   </si>
   <si>
     <t>incomplete requirements see notes: 2.1</t>
+  </si>
+  <si>
+    <t>Incorrect guess: integer. Guesses&gt;0</t>
+  </si>
+  <si>
+    <t>incorrect guess non-integer (including blank)</t>
   </si>
 </sst>
 </file>
@@ -506,7 +506,7 @@
   <dimension ref="A2:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,7 +529,7 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -617,7 +617,7 @@
         <v>2.1</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>8</v>
@@ -652,13 +652,13 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -675,7 +675,7 @@
         <v>14</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>27</v>

</xml_diff>